<commit_message>
added representants for types
</commit_message>
<xml_diff>
--- a/bwi_export2.xlsx
+++ b/bwi_export2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9bb95f21cca0349/DataChef/03_hlmd/02_wald_divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB175310-FA7B-4F50-B2E1-5872175646FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FB175310-FA7B-4F50-B2E1-5872175646FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B9E1E0CA-8568-4904-AD2B-EBB3FA10CE4E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(%)" sheetId="1" r:id="rId1"/>
@@ -355,7 +355,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1186,12 +1186,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>